<commit_message>
Completed updating all the test execution results
</commit_message>
<xml_diff>
--- a/Team 10 -Test Design Document.xlsx
+++ b/Team 10 -Test Design Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sachi\Desktop\FinalQA\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22218C75-BE87-45A9-9DA7-F46B5035829C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E1281DC8-C6A0-4E4D-8840-BC4C451C7A03}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -74,27 +74,12 @@
     <t xml:space="preserve">TC_001    </t>
   </si>
   <si>
-    <t>Team member -&gt; Enter Happiness Level</t>
-  </si>
-  <si>
-    <t>Validate that a team member can enter the individual happiness level through the application</t>
-  </si>
-  <si>
     <t>Check if the team member can select a certain happiness level to indicate the individual happiness level at a given time.</t>
   </si>
   <si>
-    <t>Check if the team member can change the initial selection of a certain happiness level before submitting the final selection.</t>
-  </si>
-  <si>
     <t>Check the Happiness Level UI requirements.</t>
   </si>
   <si>
-    <t>Check if the team member can cancel the happiness level selection without submitting the data.</t>
-  </si>
-  <si>
-    <t>Check if the selected happiness level is correctly saved when the team member submits the selection.</t>
-  </si>
-  <si>
     <t>TC_001_02</t>
   </si>
   <si>
@@ -107,70 +92,198 @@
     <t>TC_001_05</t>
   </si>
   <si>
+    <t xml:space="preserve">1. Launch the  application </t>
+  </si>
+  <si>
+    <t>TC_001_06</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
     <t>1. Launch the  application 
-2.Click on the happiness level indication images</t>
+2.Click on an individual happiness level indication image</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed.
+2_1. The team member is able to select the desired happiness level from the options
+2_2 The selection is not immediately submitted without confirmation.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Check if the team member can keep changing the initial selection of the individual happiness level before submitting the final selection.</t>
   </si>
   <si>
     <t>1. Launch the  application 
-2.Click on a happiness level indication image
-3. Click on another happiness level indication image</t>
-  </si>
-  <si>
-    <t>1. The page for entering team happiness level is displayed.
-2. The team member is able to select the desired happiness level from the list
+2.Click on an individual happiness level indication image
+3. Click on another individual happiness level indication image</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed.
+2_1 The team member is able to select the desired happiness level from the options
+2_2 The selection is not immediately submitted without confirmation.
 3_1. The team member is able to select a different desired happiness level from the list
-2_2 The selection is not immediately submitted without confirmation.</t>
-  </si>
-  <si>
-    <t>1. The page for entering team happiness level is displayed.
-2_1. The team member is able to select the desired happiness level from the list
-2_2 The selection is not immediately submitted without confirmation.</t>
-  </si>
-  <si>
-    <t>1. The page for entering team happiness level is displayed.
+3_2 The selection is not immediately submitted without confirmation.</t>
+  </si>
+  <si>
+    <t>Check if the team member can select a certain happiness level to indicate the team happiness level at a given time.</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2.Click on a team happiness level indication images</t>
+  </si>
+  <si>
+    <t>Check if the team member can keep changing the initial selection of the team happiness level before submitting the final selection.</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2.Click on a team happiness level indication image
+3. Click on another team happiness level indication image</t>
+  </si>
+  <si>
+    <t>Check if the selected happiness levels are correctly saved when the team member submits the selection.</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2.Click on an individual happiness level indication image
+2.Click on a team happiness level indication image
+3. Click on the 'Submit' button</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed.
 2_1. The team member is able to select the desired happiness level from the list
 2_2 The selection is not immediately submitted without confirmation.
-3. The selection is submitted and a confirmation message is displayed.</t>
+3_1. The team member is able to select the desired happiness level from the list
+3_2. The selection is not immediately submitted without confirmation.
+3_3. The 'Submit' button gets displyed only when both individual and team selections have been made.
+4. The selection is submitted and a confirmation message is displayed.</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed with the following UI options.
+- Happiness level indication images for individual happiness levels
+- Happiness level indication images for team happiness levels
+- Appropriate instructions messages for the two selections
+- 'Submit' button
+- Postpone links - 5 min, 10 min, 20 min</t>
+  </si>
+  <si>
+    <t>TC_001_07</t>
+  </si>
+  <si>
+    <t>Check that once the user has completed one submission, he/she is not able to resubmit another selection immediately.</t>
   </si>
   <si>
     <t>1. Launch the  application 
-2.Click on the happiness level indication images
-3. Click on the 'Submit' button</t>
-  </si>
-  <si>
-    <t>1. Launch the  application 
-2.Click on the happiness level indication images
-3. Click on the 'Cancel' button</t>
-  </si>
-  <si>
-    <t>1. The page for entering team happiness level is displayed.
+2.Click on an individual happiness level indication image
+3.Click on a team happiness level indication image
+4. Click on the 'Submit' button
+5. Click on an individual happiness level indication image
+6. Click on a team happiness level indication image</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed.
 2_1. The team member is able to select the desired happiness level from the list
 2_2 The selection is not immediately submitted without confirmation.
-3. The selection is not submitted and saved.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Launch the  application </t>
-  </si>
-  <si>
-    <t>1. The page for entering team happiness level is displayed with the following UI options.
-- Happiness level indication images for the selected number of happiness levels
-- 'Submit' button
-- 'Cancel' button</t>
-  </si>
-  <si>
-    <t>TC_001_06</t>
-  </si>
-  <si>
-    <t>Check if the order of happiness level indication images displayed are changed randomly.</t>
-  </si>
-  <si>
-    <t>1. Launch and cancel the  application mutiple times.</t>
-  </si>
-  <si>
-    <t>1. The order of images indicating happiness levels is not displayed in a consistant order.</t>
-  </si>
-  <si>
-    <t>Medium</t>
+3_1. The team member is able to select the desired happiness level from the list
+3_2. The selection is not immediately submitted without confirmation.
+3_3. The 'Submit' button gets displyed only when both individual and team selections have been made.
+4. The selection is submitted and a confirmation message is displayed.
+5. Reselection of individual happiness level is not allowed
+6. Reselection of team happiness level is not allowed</t>
+  </si>
+  <si>
+    <t>TC_002_01</t>
+  </si>
+  <si>
+    <t>Check if a desktop notification is displayed to the team member at a predefined time.</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2. Minimize the application and wait for the specified time</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed 
+2. A desktop notification is displyed indicating that it's time to enter happiness information</t>
+  </si>
+  <si>
+    <t>TC_002_02</t>
+  </si>
+  <si>
+    <t>Check if the team member can navigate to the application by clicking on the desktop notification.</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2. Minimize the application and wait for the specified time
+3. Click on the desktop notification</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed 
+2. A desktop notification is displyed indicating that it's time to enter happiness information
+3. The team member is navigated into the application to enter happiness information</t>
+  </si>
+  <si>
+    <t>TC_003_01</t>
+  </si>
+  <si>
+    <t>Check if a desktop notification is displayed to the team member after the delay time period selected by the team member. - 5 min</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2. Click on a link to postpone the notifications by 5 min
+3.Minimize the application and wait for 5 min</t>
+  </si>
+  <si>
+    <t>1. The page for entering happiness level information is displayed 
+2. A confirmation msg is displyed that the notification has been postponed
+3. A desktop notification is displyed to the team member after the specified time</t>
+  </si>
+  <si>
+    <t>TC_003_02</t>
+  </si>
+  <si>
+    <t>Check if a desktop notification is displayed to the team member after the delay time period selected by the team member. - 10 min</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2. Click on a link to postpone the notifications by 10 min
+3.Minimize the application and wait for 10 min</t>
+  </si>
+  <si>
+    <t>TC_003_03</t>
+  </si>
+  <si>
+    <t>Check if a desktop notification is displayed to the team member after the delay time period selected by the team member. - 20 min</t>
+  </si>
+  <si>
+    <t>1. Launch the  application 
+2. Click on a link to postpone the notifications by 20 min
+3.Minimize the application and wait for 20 min</t>
+  </si>
+  <si>
+    <t>Team member -&gt; Enter  Happiness Level</t>
+  </si>
+  <si>
+    <t>Validate that a team member can enter the happiness level information through the application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_002  </t>
+  </si>
+  <si>
+    <t>Team member -&gt; Desktop Notifications</t>
+  </si>
+  <si>
+    <t>Validate that a team member is displayed desktop notifications at a set time period by the admin</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>Team member -&gt; Postpone notifications through the application page</t>
+  </si>
+  <si>
+    <t>Validate that the team member can postpone a notification by 5, 10 or 20 minutes through the application page</t>
   </si>
 </sst>
 </file>
@@ -229,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -259,11 +372,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -298,17 +448,38 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,10 +798,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -684,71 +855,166 @@
       <c r="AA1" s="7"/>
     </row>
     <row r="2" spans="1:27" s="6" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>17</v>
+      <c r="B2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>20</v>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
+  <mergeCells count="9">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -760,10 +1026,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -829,166 +1095,272 @@
       <c r="AA1" s="3"/>
     </row>
     <row r="2" spans="1:27" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="G3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:27" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="13" t="s">
+      <c r="F5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:27" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:27" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:27" ht="315" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:27" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:27" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:27" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:27" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:27" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+    </row>
+    <row r="10" spans="1:27" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:27" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:27" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I5" xr:uid="{00000000-0009-0000-0000-000001000000}"/>

</xml_diff>